<commit_message>
Corrected the bug where data.extract_POV_characters() was misattributing chapters. Cause was that these chapter enteries in the spreadsheet did not close the brackets around the chapter name. Both corrected this in data set and added a check and error message to catch this in the future. Also added some explanatory comments to some of the newer code.
</commit_message>
<xml_diff>
--- a/data/1-source/03 A Storm Of Swords.xlsx
+++ b/data/1-source/03 A Storm Of Swords.xlsx
@@ -1405,7 +1405,7 @@
     <t xml:space="preserve">Lord Farman</t>
   </si>
   <si>
-    <t xml:space="preserve">CHAPTER 20 (CATELYN III</t>
+    <t xml:space="preserve">CHAPTER 20 (CATELYN III)</t>
   </si>
   <si>
     <t xml:space="preserve">Delp</t>
@@ -3248,11 +3248,11 @@
   <dimension ref="A1:AR3373"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B3128" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B699" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3128" activeCellId="0" sqref="A3128"/>
-      <selection pane="bottomRight" activeCell="E3128" activeCellId="0" sqref="E3128"/>
+      <selection pane="bottomLeft" activeCell="A699" activeCellId="0" sqref="A699"/>
+      <selection pane="bottomRight" activeCell="A781" activeCellId="1" sqref="B3160:B3161 A781"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>